<commit_message>
Fixed Base Reports Heading Displaying UpGrades
</commit_message>
<xml_diff>
--- a/Insure/UDM.Insurance.Interface/Templates/ReportTemplateDailySalesCheckingBase.xlsx
+++ b/Insure/UDM.Insurance.Interface/Templates/ReportTemplateDailySalesCheckingBase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Documents\SourceProjects\Insure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE0A75A-B275-4876-A158-112BB1231DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C514B42-8340-4A0B-A06E-21C5C64856C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1095" windowWidth="24240" windowHeight="13140" xr2:uid="{440ECAD8-9E77-4B0E-86CD-E9E348C2B6A8}"/>
   </bookViews>

</xml_diff>